<commit_message>
Signed-off-by: I Valliani <I Valliani@Valliani>
</commit_message>
<xml_diff>
--- a/ApplicationData/amazonsheet.xlsx
+++ b/ApplicationData/amazonsheet.xlsx
@@ -13,6 +13,14 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>alaxa</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,7 +367,13 @@
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>